<commit_message>
Part n of refactoring footer buttons
</commit_message>
<xml_diff>
--- a/Classeur2.xlsx
+++ b/Classeur2.xlsx
@@ -62,9 +62,6 @@
     <t>isbtnPlusDactions</t>
   </si>
   <si>
-    <t>Tant qu'on n'a pas validé final, si l'utilisateur est celui qui a saisi alors il peut close</t>
-  </si>
-  <si>
     <t>Tant qu'on n'a pas validé p ou plus, si l'utilisateur est celui qui a saisi alors il peut update</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>L'utilisateur en cours est celui qui a effectué l'action N mais celle-ci n'est plus possible parce que l'un des supérieurs a effectué l'une des actions n++</t>
   </si>
   <si>
-    <t>Si le statut est intermédiaire ( &gt;SAISI et &lt;Final) et que l'un des supérieurs n'a pas effectué l'une des actions n++</t>
-  </si>
-  <si>
     <t>Toujours</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>Si le statut est CLOT</t>
+  </si>
+  <si>
+    <t>Si le statut est intermédiaire ( &gt;SAISI et &lt;Final) et que l'utilisateur a effectué l'action de validation précédente et qu'aucun des supérieurs n'a effectué l'une des actions n++</t>
+  </si>
+  <si>
+    <t>Tant qu'on n'a pas validé final, si l'entité n'est pas close et l'utilisateur est celui qui a saisi alors il peut close</t>
   </si>
 </sst>
 </file>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -512,10 +512,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,10 +523,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,7 +534,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,10 +542,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -553,18 +553,18 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin: Handle footer button for Imputation
</commit_message>
<xml_diff>
--- a/Classeur2.xlsx
+++ b/Classeur2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>Tant qu'on n'a pas validé final, si l'entité n'est pas close et l'utilisateur est celui qui a saisi alors il peut close</t>
+  </si>
+  <si>
+    <t>isNewNextAction</t>
+  </si>
+  <si>
+    <t>Pour un engagement. Si celui-ci a un nb_imputation_encours &gt; 0 alors afficher ce bouton</t>
+  </si>
+  <si>
+    <t>Pour une imputation. Si celui-ci a un nb_apurement_encours &gt; 0 alors afficher ce bouton</t>
+  </si>
+  <si>
+    <t>Pour un apurement. Ce bouton ne s'affiche pas.</t>
   </si>
 </sst>
 </file>
@@ -149,9 +161,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +580,33 @@
         <v>17</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1) Adding methods to the imputationcard for its footer button. 2) Updating the footerbutton to handle properly nextActionButton so that a VALIDF operator can valid a VALIDP engagement. 3) Updating the createengagement Dialog to load and to be emptied after submission
</commit_message>
<xml_diff>
--- a/Classeur2.xlsx
+++ b/Classeur2.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snh\Documents\Gestion du Budget\dev\gesbudgetui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\SN\projectui\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F82F60-88EC-46DE-9664-8514D9FB226A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regles de gestion" sheetId="1" r:id="rId1"/>
+    <sheet name="TODO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -65,15 +67,6 @@
     <t>Tant qu'on n'a pas validé p ou plus, si l'utilisateur est celui qui a saisi alors il peut update</t>
   </si>
   <si>
-    <t>Si l'utilisateur en cours a le droit de Valider P et si l'utilisateur en cours n'est pas celui qui a effectué la saisie</t>
-  </si>
-  <si>
-    <t>Si l'utilisateur en cours a le droit de Valider S et si l'utilisateur en cours n'est pas celui qui a effectué la validation P</t>
-  </si>
-  <si>
-    <t>Si l'utilisateur en cours a le droit de Valider F et si l'utilisateur en cours n'est pas celui qui a effectué la validation S</t>
-  </si>
-  <si>
     <t>Si l'utilisateur en cours est celui qui a saisi et le statut est à CLOT</t>
   </si>
   <si>
@@ -120,12 +113,42 @@
   </si>
   <si>
     <t>Pour un apurement. Ce bouton ne s'affiche pas.</t>
+  </si>
+  <si>
+    <t>Apurements</t>
+  </si>
+  <si>
+    <t>Validation des formulaires</t>
+  </si>
+  <si>
+    <t>Backup journalier de la base de données.</t>
+  </si>
+  <si>
+    <t>Vue pour avoir les états des engagements par lignes budgétaire</t>
+  </si>
+  <si>
+    <t>Ajout de fichiers lors de création, imputation, apurement engagement</t>
+  </si>
+  <si>
+    <t>Si l'engagement est au statut 'VALIDP' ou 'VALIDS'. Avec l'utilisateur en cours a le droit de Valider F et si l'utilisateur en cours n'est pas celui qui a effectué la validation S</t>
+  </si>
+  <si>
+    <t>Si l'engagement est au statut 'VALIDP'. Avecl'utilisateur en cours a le droit de Valider S et si l'utilisateur en cours n'est pas celui qui a effectué la validation P</t>
+  </si>
+  <si>
+    <t>Si l'engagement est au statut 'SAISI'. Avec l'utilisateur en cours a le droit de Valider P et si l'utilisateur en cours n'est pas celui qui a effectué la saisie</t>
+  </si>
+  <si>
+    <t>Loguer les connexions</t>
+  </si>
+  <si>
+    <t>Gérer les validations, Imputations, apurement des Réalisations directes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,21 +467,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,148 +489,222 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE52165A-C4A6-4382-B2DF-0ADB759AF484}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finishing apurement feature, from creating to VALIDF
</commit_message>
<xml_diff>
--- a/Classeur2.xlsx
+++ b/Classeur2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Documents\SN\projectui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snh\Documents\Gestion du Budget\dev\gesbudgetui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F82F60-88EC-46DE-9664-8514D9FB226A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Regles de gestion" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>isbtnUpdate</t>
   </si>
@@ -118,9 +117,6 @@
     <t>Apurements</t>
   </si>
   <si>
-    <t>Validation des formulaires</t>
-  </si>
-  <si>
     <t>Backup journalier de la base de données.</t>
   </si>
   <si>
@@ -143,12 +139,21 @@
   </si>
   <si>
     <t>Gérer les validations, Imputations, apurement des Réalisations directes</t>
+  </si>
+  <si>
+    <t>Ajouter les règles de validation aux formulaires</t>
+  </si>
+  <si>
+    <t>Régularisation des imputations</t>
+  </si>
+  <si>
+    <t>Gestion des autorisation au niveau du backend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -467,21 +472,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="103.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,42 +497,42 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -535,7 +540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -543,7 +548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -554,7 +559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -565,7 +570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -573,7 +578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -584,7 +589,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -592,7 +597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -603,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -614,7 +619,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -622,7 +627,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
@@ -636,40 +641,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE52165A-C4A6-4382-B2DF-0ADB759AF484}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -677,32 +682,48 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B7">
+  <sortState ref="A1:B7">
     <sortCondition ref="A1:A7"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>